<commit_message>
Finshed testing, added add player
</commit_message>
<xml_diff>
--- a/Documentation/FUNCTIONAL_REQUIREMENTS.xlsx
+++ b/Documentation/FUNCTIONAL_REQUIREMENTS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="147">
   <si>
     <t>REQ_ID</t>
   </si>
@@ -451,14 +451,28 @@
   </si>
   <si>
     <t>The database class contains a method to get a player's average score from a particular starting point on a particular hole.</t>
+  </si>
+  <si>
+    <t>A user should be able to end a game early through an option in the action bar menu.</t>
+  </si>
+  <si>
+    <t>A user should be able to add a new player through an option in the action bar menu.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -540,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -558,7 +572,8 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -855,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M111"/>
+  <dimension ref="A1:AD113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -900,22 +915,22 @@
       </c>
     </row>
     <row r="6" spans="1:6" s="7" customFormat="1">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="14" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2296,8 +2311,11 @@
       <c r="D76" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E76" s="5" t="s">
-        <v>79</v>
+      <c r="E76" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F76" s="8">
+        <v>23</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2351,8 +2369,11 @@
       <c r="D79" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E79" s="5" t="s">
-        <v>79</v>
+      <c r="E79" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F79" s="8">
+        <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2407,6 +2428,9 @@
       <c r="E82" s="2" t="s">
         <v>114</v>
       </c>
+      <c r="F82" s="8" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="6">
@@ -2422,6 +2446,9 @@
       <c r="E83" s="2" t="s">
         <v>114</v>
       </c>
+      <c r="F83" s="8" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="6">
@@ -2456,8 +2483,11 @@
       <c r="D85" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E85" s="5" t="s">
-        <v>79</v>
+      <c r="E85" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F85" s="8">
+        <v>25</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2473,8 +2503,11 @@
       <c r="D86" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="E86" s="5" t="s">
-        <v>79</v>
+      <c r="E86" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F86" s="8">
+        <v>26</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2490,8 +2523,11 @@
       <c r="D87" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E87" s="5" t="s">
-        <v>79</v>
+      <c r="E87" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F87" s="8">
+        <v>27</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2527,8 +2563,11 @@
       <c r="D89" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E89" s="5" t="s">
-        <v>79</v>
+      <c r="E89" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F89" s="8">
+        <v>28</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2544,8 +2583,11 @@
       <c r="D90" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="E90" s="5" t="s">
-        <v>79</v>
+      <c r="E90" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F90" s="8">
+        <v>29</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2561,8 +2603,11 @@
       <c r="D91" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E91" s="5" t="s">
-        <v>79</v>
+      <c r="E91" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F91" s="8">
+        <v>30</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2663,7 +2708,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="97" spans="1:13">
+    <row r="97" spans="1:30">
       <c r="A97" s="12">
         <v>91</v>
       </c>
@@ -2681,7 +2726,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="98" spans="1:13">
+    <row r="98" spans="1:30">
       <c r="A98" s="12">
         <v>92</v>
       </c>
@@ -2699,7 +2744,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="99" spans="1:13">
+    <row r="99" spans="1:30">
       <c r="A99" s="12">
         <v>93</v>
       </c>
@@ -2717,7 +2762,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="100" spans="1:13">
+    <row r="100" spans="1:30">
       <c r="A100" s="12">
         <v>94</v>
       </c>
@@ -2735,7 +2780,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="101" spans="1:13" s="1" customFormat="1">
+    <row r="101" spans="1:30" s="1" customFormat="1">
       <c r="A101" s="6">
         <v>95</v>
       </c>
@@ -2761,8 +2806,25 @@
       <c r="K101" s="7"/>
       <c r="L101" s="7"/>
       <c r="M101" s="7"/>
-    </row>
-    <row r="102" spans="1:13">
+      <c r="N101" s="7"/>
+      <c r="O101" s="7"/>
+      <c r="P101" s="7"/>
+      <c r="Q101" s="7"/>
+      <c r="R101" s="7"/>
+      <c r="S101" s="7"/>
+      <c r="T101" s="7"/>
+      <c r="U101" s="7"/>
+      <c r="V101" s="7"/>
+      <c r="W101" s="7"/>
+      <c r="X101" s="7"/>
+      <c r="Y101" s="7"/>
+      <c r="Z101" s="7"/>
+      <c r="AA101" s="7"/>
+      <c r="AB101" s="7"/>
+      <c r="AC101" s="7"/>
+      <c r="AD101" s="7"/>
+    </row>
+    <row r="102" spans="1:30">
       <c r="A102" s="6">
         <v>96</v>
       </c>
@@ -2781,8 +2843,9 @@
       <c r="F102" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="103" spans="1:13">
+      <c r="AD102" s="7"/>
+    </row>
+    <row r="103" spans="1:30">
       <c r="A103" s="6">
         <v>97</v>
       </c>
@@ -2801,8 +2864,9 @@
       <c r="F103" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="104" spans="1:13">
+      <c r="AD103" s="7"/>
+    </row>
+    <row r="104" spans="1:30">
       <c r="A104" s="6">
         <v>98</v>
       </c>
@@ -2821,8 +2885,9 @@
       <c r="F104" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="105" spans="1:13">
+      <c r="AD104" s="7"/>
+    </row>
+    <row r="105" spans="1:30">
       <c r="A105" s="6">
         <v>99</v>
       </c>
@@ -2841,8 +2906,9 @@
       <c r="F105" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="106" spans="1:13">
+      <c r="AD105" s="7"/>
+    </row>
+    <row r="106" spans="1:30">
       <c r="A106" s="6">
         <v>100</v>
       </c>
@@ -2861,8 +2927,9 @@
       <c r="F106" s="8">
         <v>6</v>
       </c>
-    </row>
-    <row r="107" spans="1:13">
+      <c r="AD106" s="7"/>
+    </row>
+    <row r="107" spans="1:30">
       <c r="A107" s="6">
         <v>101</v>
       </c>
@@ -2881,8 +2948,9 @@
       <c r="F107" s="8">
         <v>7</v>
       </c>
-    </row>
-    <row r="108" spans="1:13">
+      <c r="AD107" s="7"/>
+    </row>
+    <row r="108" spans="1:30">
       <c r="A108" s="6">
         <v>103</v>
       </c>
@@ -2895,11 +2963,15 @@
       <c r="D108" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="E108" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="109" spans="1:13">
+      <c r="E108" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F108" s="8">
+        <v>31</v>
+      </c>
+      <c r="AD108" s="7"/>
+    </row>
+    <row r="109" spans="1:30">
       <c r="A109" s="6">
         <v>104</v>
       </c>
@@ -2918,8 +2990,9 @@
       <c r="F109" s="8">
         <v>6</v>
       </c>
-    </row>
-    <row r="110" spans="1:13">
+      <c r="AD109" s="7"/>
+    </row>
+    <row r="110" spans="1:30">
       <c r="A110" s="6">
         <v>105</v>
       </c>
@@ -2938,8 +3011,9 @@
       <c r="F110" s="8">
         <v>7</v>
       </c>
-    </row>
-    <row r="111" spans="1:13">
+      <c r="AD110" s="7"/>
+    </row>
+    <row r="111" spans="1:30">
       <c r="A111" s="6">
         <v>106</v>
       </c>
@@ -2957,6 +3031,71 @@
       </c>
       <c r="F111" s="8">
         <v>9</v>
+      </c>
+      <c r="AD111" s="7"/>
+    </row>
+    <row r="112" spans="1:30" s="3" customFormat="1">
+      <c r="A112" s="3">
+        <v>107</v>
+      </c>
+      <c r="B112" s="3">
+        <v>5</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F112" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G112" s="7"/>
+      <c r="H112" s="7"/>
+      <c r="I112" s="7"/>
+      <c r="J112" s="7"/>
+      <c r="K112" s="7"/>
+      <c r="L112" s="7"/>
+      <c r="M112" s="7"/>
+      <c r="N112" s="7"/>
+      <c r="O112" s="7"/>
+      <c r="P112" s="7"/>
+      <c r="Q112" s="7"/>
+      <c r="R112" s="7"/>
+      <c r="S112" s="7"/>
+      <c r="T112" s="7"/>
+      <c r="U112" s="7"/>
+      <c r="V112" s="7"/>
+      <c r="W112" s="7"/>
+      <c r="X112" s="7"/>
+      <c r="Y112" s="7"/>
+      <c r="Z112" s="7"/>
+      <c r="AA112" s="7"/>
+      <c r="AB112" s="7"/>
+      <c r="AC112" s="7"/>
+      <c r="AD112" s="7"/>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" s="6">
+        <v>108</v>
+      </c>
+      <c r="B113" s="6">
+        <v>4</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F113" s="8" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more testing, minor functionalty changes
</commit_message>
<xml_diff>
--- a/Documentation/FUNCTIONAL_REQUIREMENTS.xlsx
+++ b/Documentation/FUNCTIONAL_REQUIREMENTS.xlsx
@@ -273,9 +273,6 @@
     <t>Class: Hole</t>
   </si>
   <si>
-    <t>The Hole class exists. It has a holenUmber, a par, and a list of HoleStartingPoints. It is parcelable.</t>
-  </si>
-  <si>
     <t>The Hole class contains a method for getting all of its starting point names as a list of strings.</t>
   </si>
   <si>
@@ -457,6 +454,9 @@
   </si>
   <si>
     <t>A user should be able to add a new player through an option in the action bar menu.</t>
+  </si>
+  <si>
+    <t>The Hole class exists. It has a holeNumber, a par, and a list of HoleStartingPoints. It is parcelable.</t>
   </si>
 </sst>
 </file>
@@ -872,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -903,7 +903,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="D3" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>80</v>
@@ -911,7 +911,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="E4" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="7" customFormat="1">
@@ -925,7 +925,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>3</v>
@@ -946,10 +946,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -964,10 +964,10 @@
         <v>7</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -982,10 +982,10 @@
         <v>17</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1000,10 +1000,10 @@
         <v>16</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1018,10 +1018,10 @@
         <v>6</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1038,10 +1038,10 @@
         <v>9</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1058,10 +1058,10 @@
         <v>10</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1078,10 +1078,10 @@
         <v>12</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1098,10 +1098,10 @@
         <v>13</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1118,10 +1118,10 @@
         <v>14</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1138,10 +1138,10 @@
         <v>15</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1158,10 +1158,10 @@
         <v>19</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1178,10 +1178,10 @@
         <v>20</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1198,10 +1198,10 @@
         <v>21</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1218,10 +1218,10 @@
         <v>23</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1238,10 +1238,10 @@
         <v>24</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1258,10 +1258,10 @@
         <v>25</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1278,10 +1278,10 @@
         <v>26</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1298,10 +1298,10 @@
         <v>27</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1318,10 +1318,10 @@
         <v>28</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1338,10 +1338,10 @@
         <v>29</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1358,10 +1358,10 @@
         <v>30</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1378,10 +1378,10 @@
         <v>31</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1396,10 +1396,10 @@
         <v>32</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1416,10 +1416,10 @@
         <v>34</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1436,10 +1436,10 @@
         <v>35</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1454,10 +1454,10 @@
         <v>38</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1474,10 +1474,10 @@
         <v>39</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1494,10 +1494,10 @@
         <v>40</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1514,10 +1514,10 @@
         <v>42</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1534,10 +1534,10 @@
         <v>43</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1554,10 +1554,10 @@
         <v>44</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1574,10 +1574,10 @@
         <v>45</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1594,10 +1594,10 @@
         <v>46</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1614,10 +1614,10 @@
         <v>47</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2031,7 +2031,7 @@
         <v>37</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>78</v>
@@ -2051,7 +2051,7 @@
         <v>37</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>78</v>
@@ -2212,10 +2212,10 @@
         <v>83</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="72" spans="1:6" s="7" customFormat="1">
@@ -2229,13 +2229,13 @@
         <v>84</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2249,7 +2249,7 @@
         <v>84</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>78</v>
@@ -2269,7 +2269,7 @@
         <v>84</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>78</v>
@@ -2289,13 +2289,13 @@
         <v>36</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2309,7 +2309,7 @@
         <v>36</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>78</v>
@@ -2324,16 +2324,16 @@
       </c>
       <c r="B77" s="6"/>
       <c r="C77" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D77" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D77" s="6" t="s">
-        <v>91</v>
-      </c>
       <c r="E77" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F77" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2341,19 +2341,19 @@
         <v>72</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C78" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D78" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D78" s="6" t="s">
-        <v>93</v>
-      </c>
       <c r="E78" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F78" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2364,10 +2364,10 @@
         <v>72</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>78</v>
@@ -2381,19 +2381,19 @@
         <v>74</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C80" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D80" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D80" s="6" t="s">
-        <v>97</v>
-      </c>
       <c r="E80" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F80" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2402,16 +2402,16 @@
       </c>
       <c r="B81" s="6"/>
       <c r="C81" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D81" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D81" s="6" t="s">
-        <v>100</v>
-      </c>
       <c r="E81" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F81" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2420,16 +2420,16 @@
       </c>
       <c r="B82" s="6"/>
       <c r="C82" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F82" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2438,16 +2438,16 @@
       </c>
       <c r="B83" s="6"/>
       <c r="C83" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F83" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2458,16 +2458,16 @@
         <v>71</v>
       </c>
       <c r="C84" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D84" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D84" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="E84" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F84" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2478,10 +2478,10 @@
         <v>78</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>78</v>
@@ -2498,10 +2498,10 @@
         <v>78</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E86" s="4" t="s">
         <v>78</v>
@@ -2518,10 +2518,10 @@
         <v>78</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>78</v>
@@ -2538,16 +2538,16 @@
         <v>69</v>
       </c>
       <c r="C88" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D88" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D88" s="6" t="s">
-        <v>109</v>
-      </c>
       <c r="E88" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F88" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2558,10 +2558,10 @@
         <v>82</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>78</v>
@@ -2578,10 +2578,10 @@
         <v>82</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>78</v>
@@ -2598,10 +2598,10 @@
         <v>82</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E91" s="4" t="s">
         <v>78</v>
@@ -2616,16 +2616,16 @@
       </c>
       <c r="B92" s="3"/>
       <c r="C92" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E92" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D92" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="F92" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -2636,16 +2636,16 @@
         <v>86</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E93" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F93" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2656,16 +2656,16 @@
         <v>86</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E94" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F94" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2676,16 +2676,16 @@
         <v>86</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E95" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F95" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2696,16 +2696,16 @@
         <v>86</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E96" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F96" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="97" spans="1:30">
@@ -2714,16 +2714,16 @@
       </c>
       <c r="B97" s="12"/>
       <c r="C97" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D97" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="D97" s="12" t="s">
-        <v>124</v>
-      </c>
       <c r="E97" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="98" spans="1:30">
@@ -2732,16 +2732,16 @@
       </c>
       <c r="B98" s="12"/>
       <c r="C98" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E98" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F98" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="99" spans="1:30">
@@ -2753,13 +2753,13 @@
         <v>22</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E99" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="100" spans="1:30">
@@ -2768,16 +2768,16 @@
       </c>
       <c r="B100" s="12"/>
       <c r="C100" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D100" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="D100" s="12" t="s">
-        <v>128</v>
-      </c>
       <c r="E100" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="101" spans="1:30" s="1" customFormat="1">
@@ -2788,10 +2788,10 @@
         <v>27</v>
       </c>
       <c r="C101" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D101" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="D101" s="6" t="s">
-        <v>130</v>
       </c>
       <c r="E101" s="4" t="s">
         <v>78</v>
@@ -2835,7 +2835,7 @@
         <v>37</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E102" s="4" t="s">
         <v>78</v>
@@ -2856,7 +2856,7 @@
         <v>37</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>78</v>
@@ -2877,7 +2877,7 @@
         <v>37</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E104" s="4" t="s">
         <v>78</v>
@@ -2898,7 +2898,7 @@
         <v>37</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E105" s="4" t="s">
         <v>78</v>
@@ -2919,7 +2919,7 @@
         <v>37</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E106" s="4" t="s">
         <v>78</v>
@@ -2940,7 +2940,7 @@
         <v>37</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E107" s="4" t="s">
         <v>78</v>
@@ -2961,7 +2961,7 @@
         <v>37</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E108" s="4" t="s">
         <v>78</v>
@@ -2982,7 +2982,7 @@
         <v>37</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E109" s="4" t="s">
         <v>78</v>
@@ -3003,7 +3003,7 @@
         <v>37</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E110" s="4" t="s">
         <v>78</v>
@@ -3021,10 +3021,10 @@
         <v>27</v>
       </c>
       <c r="C111" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D111" s="6" t="s">
         <v>141</v>
-      </c>
-      <c r="D111" s="6" t="s">
-        <v>142</v>
       </c>
       <c r="E111" s="4" t="s">
         <v>78</v>
@@ -3035,23 +3035,23 @@
       <c r="AD111" s="7"/>
     </row>
     <row r="112" spans="1:30" s="3" customFormat="1">
-      <c r="A112" s="3">
+      <c r="A112" s="6">
         <v>107</v>
       </c>
-      <c r="B112" s="3">
+      <c r="B112" s="6">
         <v>5</v>
       </c>
-      <c r="C112" s="3" t="s">
+      <c r="C112" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D112" s="3" t="s">
-        <v>145</v>
+      <c r="D112" s="6" t="s">
+        <v>144</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F112" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G112" s="7"/>
       <c r="H112" s="7"/>
@@ -3089,13 +3089,13 @@
         <v>18</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F113" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added asynchronous calls in multiple activities
</commit_message>
<xml_diff>
--- a/Documentation/FUNCTIONAL_REQUIREMENTS.xlsx
+++ b/Documentation/FUNCTIONAL_REQUIREMENTS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="169">
   <si>
     <t>REQ_ID</t>
   </si>
@@ -457,13 +457,79 @@
   </si>
   <si>
     <t>The Hole class exists. It has a holeNumber, a par, and a list of HoleStartingPoints. It is parcelable.</t>
+  </si>
+  <si>
+    <t>Class: Game</t>
+  </si>
+  <si>
+    <t>The Game class should exist, it had an id, a Course, a PlayerList, a List of HoleScoreLists, and a courseScoreList.</t>
+  </si>
+  <si>
+    <t>The Game class should have methods for getting the next and previos HoleScore List.</t>
+  </si>
+  <si>
+    <t>The Game class should have a method for getting a players score for the current hole.</t>
+  </si>
+  <si>
+    <t>The Game class should have methods for incrementing and decrementing a player's course score.</t>
+  </si>
+  <si>
+    <t>The Game class should have a method for getting a player's current course score.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Game class should have a method for checking whether a hole is the last hole in a course. </t>
+  </si>
+  <si>
+    <t>Activity: Statistics</t>
+  </si>
+  <si>
+    <t>The statistics activity exists and is accessible from the home menu.</t>
+  </si>
+  <si>
+    <t>Statistics: User-Interface</t>
+  </si>
+  <si>
+    <t>The user can choose between Game History, Player Statistics, or Course Statistics.</t>
+  </si>
+  <si>
+    <t>Statistics: GameHistory Act.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The GameHistory Activity is acessible from the statistics menu. </t>
+  </si>
+  <si>
+    <t>GameHistory Activity</t>
+  </si>
+  <si>
+    <t>The GameHistory Activity has a Listview of games from the databse to choose from.</t>
+  </si>
+  <si>
+    <t>GameStats Activity</t>
+  </si>
+  <si>
+    <t>The GameStats activity is launched by clicking a game in the GameHistory activity.</t>
+  </si>
+  <si>
+    <t>Shows Course, date, and overall player scores at top of activity.</t>
+  </si>
+  <si>
+    <t>Has a Listview of Holes that were played in the course.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When hole is clicked in listview, it expands to show player's scores on the hole. </t>
+  </si>
+  <si>
+    <t>PlayGame: Backend</t>
+  </si>
+  <si>
+    <t>Make database call to insert game asynchronous.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,6 +540,36 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -554,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -575,6 +671,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -870,10 +982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD113"/>
+  <dimension ref="A1:AD128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D122" sqref="D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -883,9 +995,22 @@
     <col min="4" max="4" width="156.85546875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" style="8" customWidth="1"/>
+    <col min="13" max="13" width="4" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" customWidth="1"/>
+    <col min="15" max="15" width="5" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" customWidth="1"/>
+    <col min="17" max="17" width="6.85546875" customWidth="1"/>
+    <col min="18" max="18" width="8.5703125" customWidth="1"/>
+    <col min="19" max="19" width="17.28515625" customWidth="1"/>
+    <col min="20" max="20" width="116.28515625" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" customWidth="1"/>
+    <col min="24" max="24" width="2.140625" customWidth="1"/>
+    <col min="25" max="26" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="1" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:29">
       <c r="D1" s="6" t="s">
         <v>76</v>
       </c>
@@ -893,7 +1018,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:29">
       <c r="D2" s="3" t="s">
         <v>77</v>
       </c>
@@ -901,7 +1026,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:29">
       <c r="D3" s="10" t="s">
         <v>121</v>
       </c>
@@ -909,12 +1034,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:29">
       <c r="E4" s="11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="7" customFormat="1">
+    <row r="6" spans="1:29" s="7" customFormat="1">
       <c r="A6" s="13" t="s">
         <v>0</v>
       </c>
@@ -933,8 +1058,26 @@
       <c r="F6" s="14" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="L6" s="15"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="15"/>
+    </row>
+    <row r="7" spans="1:29">
       <c r="A7" s="6">
         <v>1</v>
       </c>
@@ -951,8 +1094,26 @@
       <c r="F7" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="L7" s="17"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="18"/>
+      <c r="Z7" s="18"/>
+      <c r="AA7" s="18"/>
+      <c r="AB7" s="18"/>
+      <c r="AC7" s="17"/>
+    </row>
+    <row r="8" spans="1:29">
       <c r="A8" s="6">
         <v>2</v>
       </c>
@@ -969,8 +1130,26 @@
       <c r="F8" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="L8" s="17"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="18"/>
+      <c r="AA8" s="18"/>
+      <c r="AB8" s="18"/>
+      <c r="AC8" s="17"/>
+    </row>
+    <row r="9" spans="1:29">
       <c r="A9" s="6">
         <v>3</v>
       </c>
@@ -987,8 +1166,26 @@
       <c r="F9" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="L9" s="17"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="18"/>
+      <c r="Z9" s="18"/>
+      <c r="AA9" s="18"/>
+      <c r="AB9" s="18"/>
+      <c r="AC9" s="17"/>
+    </row>
+    <row r="10" spans="1:29">
       <c r="A10" s="6">
         <v>4</v>
       </c>
@@ -1005,8 +1202,26 @@
       <c r="F10" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="L10" s="17"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="18"/>
+      <c r="Z10" s="18"/>
+      <c r="AA10" s="18"/>
+      <c r="AB10" s="18"/>
+      <c r="AC10" s="17"/>
+    </row>
+    <row r="11" spans="1:29">
       <c r="A11" s="6">
         <v>5</v>
       </c>
@@ -1023,8 +1238,26 @@
       <c r="F11" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="L11" s="17"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="18"/>
+      <c r="Z11" s="18"/>
+      <c r="AA11" s="18"/>
+      <c r="AB11" s="18"/>
+      <c r="AC11" s="17"/>
+    </row>
+    <row r="12" spans="1:29">
       <c r="A12" s="6">
         <v>6</v>
       </c>
@@ -1043,8 +1276,26 @@
       <c r="F12" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="17"/>
+      <c r="Y12" s="17"/>
+      <c r="Z12" s="17"/>
+      <c r="AA12" s="17"/>
+      <c r="AB12" s="17"/>
+      <c r="AC12" s="17"/>
+    </row>
+    <row r="13" spans="1:29">
       <c r="A13" s="6">
         <v>7</v>
       </c>
@@ -1063,8 +1314,16 @@
       <c r="F13" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+    </row>
+    <row r="14" spans="1:29">
       <c r="A14" s="6">
         <v>8</v>
       </c>
@@ -1083,8 +1342,16 @@
       <c r="F14" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
+    </row>
+    <row r="15" spans="1:29">
       <c r="A15" s="6">
         <v>9</v>
       </c>
@@ -1103,8 +1370,16 @@
       <c r="F15" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
+    </row>
+    <row r="16" spans="1:29">
       <c r="A16" s="6">
         <v>10</v>
       </c>
@@ -1123,8 +1398,16 @@
       <c r="F16" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="21"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17" s="6">
         <v>11</v>
       </c>
@@ -1143,8 +1426,16 @@
       <c r="F17" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+    </row>
+    <row r="18" spans="1:22">
       <c r="A18" s="6">
         <v>12</v>
       </c>
@@ -1163,8 +1454,16 @@
       <c r="F18" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+    </row>
+    <row r="19" spans="1:22">
       <c r="A19" s="6">
         <v>13</v>
       </c>
@@ -1183,8 +1482,16 @@
       <c r="F19" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="20"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="22"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+    </row>
+    <row r="20" spans="1:22">
       <c r="A20" s="6">
         <v>14</v>
       </c>
@@ -1203,8 +1510,16 @@
       <c r="F20" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="20"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="22"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+    </row>
+    <row r="21" spans="1:22">
       <c r="A21" s="6">
         <v>15</v>
       </c>
@@ -1223,8 +1538,16 @@
       <c r="F21" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="20"/>
+      <c r="S21" s="22"/>
+      <c r="T21" s="22"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="7"/>
+    </row>
+    <row r="22" spans="1:22">
       <c r="A22" s="6">
         <v>16</v>
       </c>
@@ -1243,8 +1566,16 @@
       <c r="F22" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="20"/>
+      <c r="S22" s="22"/>
+      <c r="T22" s="22"/>
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
+    </row>
+    <row r="23" spans="1:22">
       <c r="A23" s="6">
         <v>17</v>
       </c>
@@ -1263,8 +1594,16 @@
       <c r="F23" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="20"/>
+      <c r="S23" s="22"/>
+      <c r="T23" s="22"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+    </row>
+    <row r="24" spans="1:22">
       <c r="A24" s="6">
         <v>18</v>
       </c>
@@ -1283,8 +1622,16 @@
       <c r="F24" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="20"/>
+      <c r="S24" s="22"/>
+      <c r="T24" s="22"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+    </row>
+    <row r="25" spans="1:22">
       <c r="A25" s="6">
         <v>19</v>
       </c>
@@ -1303,8 +1650,16 @@
       <c r="F25" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="20"/>
+      <c r="S25" s="22"/>
+      <c r="T25" s="22"/>
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
+    </row>
+    <row r="26" spans="1:22">
       <c r="A26" s="6">
         <v>20</v>
       </c>
@@ -1323,8 +1678,16 @@
       <c r="F26" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="20"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="22"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
+    </row>
+    <row r="27" spans="1:22">
       <c r="A27" s="6">
         <v>21</v>
       </c>
@@ -1343,8 +1706,16 @@
       <c r="F27" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="20"/>
+      <c r="R27" s="20"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22"/>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
+    </row>
+    <row r="28" spans="1:22">
       <c r="A28" s="6">
         <v>22</v>
       </c>
@@ -1363,8 +1734,16 @@
       <c r="F28" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="20"/>
+      <c r="R28" s="20"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
+      <c r="U28" s="7"/>
+      <c r="V28" s="7"/>
+    </row>
+    <row r="29" spans="1:22">
       <c r="A29" s="6">
         <v>23</v>
       </c>
@@ -1383,8 +1762,16 @@
       <c r="F29" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="20"/>
+      <c r="R29" s="20"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="22"/>
+      <c r="U29" s="7"/>
+      <c r="V29" s="7"/>
+    </row>
+    <row r="30" spans="1:22">
       <c r="A30" s="6">
         <v>24</v>
       </c>
@@ -1401,8 +1788,16 @@
       <c r="F30" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="20"/>
+      <c r="R30" s="20"/>
+      <c r="S30" s="22"/>
+      <c r="T30" s="22"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
+    </row>
+    <row r="31" spans="1:22">
       <c r="A31" s="6">
         <v>25</v>
       </c>
@@ -1421,8 +1816,16 @@
       <c r="F31" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="20"/>
+      <c r="R31" s="20"/>
+      <c r="S31" s="22"/>
+      <c r="T31" s="22"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7"/>
+    </row>
+    <row r="32" spans="1:22">
       <c r="A32" s="6">
         <v>26</v>
       </c>
@@ -1441,8 +1844,16 @@
       <c r="F32" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="20"/>
+      <c r="R32" s="20"/>
+      <c r="S32" s="22"/>
+      <c r="T32" s="22"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="7"/>
+    </row>
+    <row r="33" spans="1:22">
       <c r="A33" s="6">
         <v>27</v>
       </c>
@@ -1459,8 +1870,16 @@
       <c r="F33" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="20"/>
+      <c r="R33" s="20"/>
+      <c r="S33" s="22"/>
+      <c r="T33" s="22"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+    </row>
+    <row r="34" spans="1:22">
       <c r="A34" s="6">
         <v>28</v>
       </c>
@@ -1479,8 +1898,16 @@
       <c r="F34" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="20"/>
+      <c r="R34" s="20"/>
+      <c r="S34" s="22"/>
+      <c r="T34" s="22"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
+    </row>
+    <row r="35" spans="1:22">
       <c r="A35" s="6">
         <v>29</v>
       </c>
@@ -1499,8 +1926,16 @@
       <c r="F35" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="20"/>
+      <c r="R35" s="20"/>
+      <c r="S35" s="22"/>
+      <c r="T35" s="22"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
+    </row>
+    <row r="36" spans="1:22">
       <c r="A36" s="6">
         <v>30</v>
       </c>
@@ -1519,8 +1954,16 @@
       <c r="F36" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7"/>
+    </row>
+    <row r="37" spans="1:22">
       <c r="A37" s="6">
         <v>31</v>
       </c>
@@ -1539,8 +1982,16 @@
       <c r="F37" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
+      <c r="U37" s="7"/>
+      <c r="V37" s="7"/>
+    </row>
+    <row r="38" spans="1:22">
       <c r="A38" s="6">
         <v>32</v>
       </c>
@@ -1559,8 +2010,16 @@
       <c r="F38" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="7"/>
+      <c r="U38" s="7"/>
+      <c r="V38" s="7"/>
+    </row>
+    <row r="39" spans="1:22">
       <c r="A39" s="6">
         <v>33</v>
       </c>
@@ -1579,8 +2038,16 @@
       <c r="F39" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
+      <c r="U39" s="7"/>
+      <c r="V39" s="7"/>
+    </row>
+    <row r="40" spans="1:22">
       <c r="A40" s="6">
         <v>34</v>
       </c>
@@ -1600,7 +2067,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:22">
       <c r="A41" s="6">
         <v>35</v>
       </c>
@@ -1620,7 +2087,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:22">
       <c r="A42" s="6">
         <v>36</v>
       </c>
@@ -1640,7 +2107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:22">
       <c r="A43" s="6">
         <v>37</v>
       </c>
@@ -1660,7 +2127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:22">
       <c r="A44" s="6">
         <v>38</v>
       </c>
@@ -1680,7 +2147,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:22">
       <c r="A45" s="6">
         <v>39</v>
       </c>
@@ -1700,7 +2167,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:22">
       <c r="A46" s="6">
         <v>40</v>
       </c>
@@ -1720,7 +2187,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:22">
       <c r="A47" s="6">
         <v>41</v>
       </c>
@@ -1740,7 +2207,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:22">
       <c r="A48" s="6">
         <v>42</v>
       </c>
@@ -3096,6 +3563,241 @@
       </c>
       <c r="F113" s="8" t="s">
         <v>115</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114" s="6">
+        <v>109</v>
+      </c>
+      <c r="B114" s="6"/>
+      <c r="C114" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F114" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" s="6">
+        <v>110</v>
+      </c>
+      <c r="B115" s="6">
+        <v>109</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E115" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F115" s="8">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116" s="6">
+        <v>112</v>
+      </c>
+      <c r="B116" s="6">
+        <v>109</v>
+      </c>
+      <c r="C116" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D116" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F116" s="8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117" s="6">
+        <v>113</v>
+      </c>
+      <c r="B117" s="6">
+        <v>109</v>
+      </c>
+      <c r="C117" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D117" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F117" s="8">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118" s="6">
+        <v>114</v>
+      </c>
+      <c r="B118" s="6">
+        <v>109</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D118" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F118" s="8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119" s="6">
+        <v>115</v>
+      </c>
+      <c r="B119" s="6">
+        <v>109</v>
+      </c>
+      <c r="C119" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D119" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E119" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="A120">
+        <v>116</v>
+      </c>
+      <c r="C120" t="s">
+        <v>154</v>
+      </c>
+      <c r="D120" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121">
+        <v>117</v>
+      </c>
+      <c r="B121">
+        <v>116</v>
+      </c>
+      <c r="C121" t="s">
+        <v>156</v>
+      </c>
+      <c r="D121" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122">
+        <v>118</v>
+      </c>
+      <c r="B122">
+        <v>116</v>
+      </c>
+      <c r="C122" t="s">
+        <v>158</v>
+      </c>
+      <c r="D122" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123">
+        <v>119</v>
+      </c>
+      <c r="B123">
+        <v>116</v>
+      </c>
+      <c r="C123" t="s">
+        <v>160</v>
+      </c>
+      <c r="D123" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124">
+        <v>120</v>
+      </c>
+      <c r="B124">
+        <v>119</v>
+      </c>
+      <c r="C124" t="s">
+        <v>162</v>
+      </c>
+      <c r="D124" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125">
+        <v>121</v>
+      </c>
+      <c r="B125">
+        <v>120</v>
+      </c>
+      <c r="C125" t="s">
+        <v>162</v>
+      </c>
+      <c r="D125" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126">
+        <v>122</v>
+      </c>
+      <c r="B126">
+        <v>120</v>
+      </c>
+      <c r="C126" t="s">
+        <v>162</v>
+      </c>
+      <c r="D126" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127">
+        <v>123</v>
+      </c>
+      <c r="B127">
+        <v>120</v>
+      </c>
+      <c r="C127" t="s">
+        <v>162</v>
+      </c>
+      <c r="D127" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128">
+        <v>124</v>
+      </c>
+      <c r="C128" t="s">
+        <v>167</v>
+      </c>
+      <c r="D128" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added basic parts of statistics functionality, game stats
</commit_message>
<xml_diff>
--- a/Documentation/FUNCTIONAL_REQUIREMENTS.xlsx
+++ b/Documentation/FUNCTIONAL_REQUIREMENTS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="171">
   <si>
     <t>REQ_ID</t>
   </si>
@@ -462,9 +462,6 @@
     <t>Class: Game</t>
   </si>
   <si>
-    <t>The Game class should exist, it had an id, a Course, a PlayerList, a List of HoleScoreLists, and a courseScoreList.</t>
-  </si>
-  <si>
     <t>The Game class should have methods for getting the next and previos HoleScore List.</t>
   </si>
   <si>
@@ -523,6 +520,15 @@
   </si>
   <si>
     <t>Make database call to insert game asynchronous.</t>
+  </si>
+  <si>
+    <t>Add Cancel Game option to actionbar menu, which cancels a game early without saving its data into the database.</t>
+  </si>
+  <si>
+    <t>Add Skip Hole option to actionbar menu, so a player can skip a hole without affecting their statistics.</t>
+  </si>
+  <si>
+    <t>The Game class should exist, it had an id, a Course, a PlayerList, a List of HoleScoreLists, and a courseScoreList. The Class is also Parcelable.</t>
   </si>
 </sst>
 </file>
@@ -982,10 +988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD128"/>
+  <dimension ref="A1:AD130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D122" sqref="D122"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3078,14 +3084,14 @@
       </c>
     </row>
     <row r="92" spans="1:6">
-      <c r="A92" s="3">
+      <c r="A92" s="12">
         <v>86</v>
       </c>
-      <c r="B92" s="3"/>
-      <c r="C92" s="3" t="s">
+      <c r="B92" s="12"/>
+      <c r="C92" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D92" s="3" t="s">
+      <c r="D92" s="12" t="s">
         <v>116</v>
       </c>
       <c r="E92" s="2" t="s">
@@ -3096,16 +3102,16 @@
       </c>
     </row>
     <row r="93" spans="1:6">
-      <c r="A93" s="3">
+      <c r="A93" s="12">
         <v>87</v>
       </c>
-      <c r="B93" s="3">
+      <c r="B93" s="12">
         <v>86</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C93" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D93" s="3" t="s">
+      <c r="D93" s="12" t="s">
         <v>117</v>
       </c>
       <c r="E93" s="11" t="s">
@@ -3116,16 +3122,16 @@
       </c>
     </row>
     <row r="94" spans="1:6">
-      <c r="A94" s="3">
+      <c r="A94" s="12">
         <v>88</v>
       </c>
-      <c r="B94" s="3">
+      <c r="B94" s="12">
         <v>86</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="C94" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D94" s="3" t="s">
+      <c r="D94" s="12" t="s">
         <v>118</v>
       </c>
       <c r="E94" s="11" t="s">
@@ -3136,16 +3142,16 @@
       </c>
     </row>
     <row r="95" spans="1:6">
-      <c r="A95" s="3">
+      <c r="A95" s="12">
         <v>89</v>
       </c>
-      <c r="B95" s="3">
+      <c r="B95" s="12">
         <v>86</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="C95" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D95" s="3" t="s">
+      <c r="D95" s="12" t="s">
         <v>119</v>
       </c>
       <c r="E95" s="11" t="s">
@@ -3156,16 +3162,16 @@
       </c>
     </row>
     <row r="96" spans="1:6">
-      <c r="A96" s="3">
+      <c r="A96" s="12">
         <v>90</v>
       </c>
-      <c r="B96" s="3">
+      <c r="B96" s="12">
         <v>86</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="C96" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="D96" s="12" t="s">
         <v>120</v>
       </c>
       <c r="E96" s="11" t="s">
@@ -3574,7 +3580,7 @@
         <v>147</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>113</v>
@@ -3594,7 +3600,7 @@
         <v>147</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E115" s="5" t="s">
         <v>79</v>
@@ -3614,7 +3620,7 @@
         <v>147</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E116" s="5" t="s">
         <v>79</v>
@@ -3634,7 +3640,7 @@
         <v>147</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E117" s="5" t="s">
         <v>79</v>
@@ -3654,7 +3660,7 @@
         <v>147</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E118" s="5" t="s">
         <v>79</v>
@@ -3674,77 +3680,78 @@
         <v>147</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E119" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="120" spans="1:6">
-      <c r="A120">
+      <c r="A120" s="6">
         <v>116</v>
       </c>
-      <c r="C120" t="s">
+      <c r="B120" s="6"/>
+      <c r="C120" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D120" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="D120" t="s">
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121" s="6">
+        <v>117</v>
+      </c>
+      <c r="B121" s="6">
+        <v>116</v>
+      </c>
+      <c r="C121" s="6" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="121" spans="1:6">
-      <c r="A121">
-        <v>117</v>
-      </c>
-      <c r="B121">
+      <c r="D121" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" s="6">
+        <v>118</v>
+      </c>
+      <c r="B122" s="6">
         <v>116</v>
       </c>
-      <c r="C121" t="s">
-        <v>156</v>
-      </c>
-      <c r="D121" t="s">
+      <c r="C122" s="6" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="122" spans="1:6">
-      <c r="A122">
-        <v>118</v>
-      </c>
-      <c r="B122">
+      <c r="D122" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" s="6">
+        <v>119</v>
+      </c>
+      <c r="B123" s="6">
         <v>116</v>
       </c>
-      <c r="C122" t="s">
-        <v>158</v>
-      </c>
-      <c r="D122" t="s">
+      <c r="C123" s="6" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="123" spans="1:6">
-      <c r="A123">
+      <c r="D123" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" s="6">
+        <v>120</v>
+      </c>
+      <c r="B124" s="6">
         <v>119</v>
       </c>
-      <c r="B123">
-        <v>116</v>
-      </c>
-      <c r="C123" t="s">
-        <v>160</v>
-      </c>
-      <c r="D123" t="s">
+      <c r="C124" s="6" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="124" spans="1:6">
-      <c r="A124">
-        <v>120</v>
-      </c>
-      <c r="B124">
-        <v>119</v>
-      </c>
-      <c r="C124" t="s">
+      <c r="D124" s="6" t="s">
         <v>162</v>
-      </c>
-      <c r="D124" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -3755,10 +3762,10 @@
         <v>120</v>
       </c>
       <c r="C125" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D125" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -3769,10 +3776,10 @@
         <v>120</v>
       </c>
       <c r="C126" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D126" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -3783,21 +3790,58 @@
         <v>120</v>
       </c>
       <c r="C127" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D127" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" s="6">
+        <v>124</v>
+      </c>
+      <c r="B128" s="6">
+        <v>5</v>
+      </c>
+      <c r="C128" s="6" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="128" spans="1:6">
-      <c r="A128">
-        <v>124</v>
-      </c>
-      <c r="C128" t="s">
+      <c r="D128" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="D128" t="s">
+      <c r="E128" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F128" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129">
+        <v>125</v>
+      </c>
+      <c r="B129">
+        <v>5</v>
+      </c>
+      <c r="C129" t="s">
+        <v>22</v>
+      </c>
+      <c r="D129" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130">
+        <v>126</v>
+      </c>
+      <c r="B130">
+        <v>5</v>
+      </c>
+      <c r="C130" t="s">
+        <v>22</v>
+      </c>
+      <c r="D130" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new course, menu changes.
</commit_message>
<xml_diff>
--- a/Documentation/FUNCTIONAL_REQUIREMENTS.xlsx
+++ b/Documentation/FUNCTIONAL_REQUIREMENTS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="182">
   <si>
     <t>REQ_ID</t>
   </si>
@@ -529,6 +529,39 @@
   </si>
   <si>
     <t>The Game class should exist, it had an id, a Course, a PlayerList, a List of HoleScoreLists, and a courseScoreList. The Class is also Parcelable.</t>
+  </si>
+  <si>
+    <t>The DB class contains a method for getting all of the holescores for a particular game.</t>
+  </si>
+  <si>
+    <t>The DB class contains a method for getting all of the holescores for a particular hole.</t>
+  </si>
+  <si>
+    <t>Activity: Add Course</t>
+  </si>
+  <si>
+    <t>An Activity exists for adding a course into the database.</t>
+  </si>
+  <si>
+    <t>Add Course: User Interface</t>
+  </si>
+  <si>
+    <t>Has an edittext for typing the course name</t>
+  </si>
+  <si>
+    <t>Has an edittext for entering the city the course is in.</t>
+  </si>
+  <si>
+    <t>Has a selector for selecting the number of holes the course has.</t>
+  </si>
+  <si>
+    <t>Play Game: User Interface</t>
+  </si>
+  <si>
+    <t>Can drop a player from the current game. Player stats should be saved.</t>
+  </si>
+  <si>
+    <t>Has a edittext for entering state the course is in.</t>
   </si>
 </sst>
 </file>
@@ -988,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD130"/>
+  <dimension ref="A1:AD138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D140" sqref="D140"/>
+    <sheetView tabSelected="1" topLeftCell="B118" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3820,13 +3853,13 @@
       <c r="A129">
         <v>125</v>
       </c>
-      <c r="B129">
+      <c r="B129" s="6">
         <v>5</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C129" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D129" s="6" t="s">
         <v>168</v>
       </c>
     </row>
@@ -3842,6 +3875,108 @@
       </c>
       <c r="D130" t="s">
         <v>169</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131">
+        <v>127</v>
+      </c>
+      <c r="B131">
+        <v>27</v>
+      </c>
+      <c r="C131" t="s">
+        <v>37</v>
+      </c>
+      <c r="D131" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132">
+        <v>128</v>
+      </c>
+      <c r="B132">
+        <v>27</v>
+      </c>
+      <c r="C132" t="s">
+        <v>37</v>
+      </c>
+      <c r="D132" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133">
+        <v>129</v>
+      </c>
+      <c r="B133" s="6"/>
+      <c r="C133" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D133" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134">
+        <v>130</v>
+      </c>
+      <c r="B134" s="6"/>
+      <c r="C134" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D134" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135">
+        <v>131</v>
+      </c>
+      <c r="B135" s="6"/>
+      <c r="C135" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D135" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136">
+        <v>132</v>
+      </c>
+      <c r="B136" s="6"/>
+      <c r="C136" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D136" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137">
+        <v>133</v>
+      </c>
+      <c r="B137" s="6"/>
+      <c r="C137" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D137" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138">
+        <v>134</v>
+      </c>
+      <c r="B138" s="6">
+        <v>5</v>
+      </c>
+      <c r="C138" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="D138" s="6" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>